<commit_message>
update last adding customer in penjualan
</commit_message>
<xml_diff>
--- a/Raw Process New Modul_.xlsx
+++ b/Raw Process New Modul_.xlsx
@@ -123,6 +123,10 @@
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #000000"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0pt"/>
     </style:style>
+    <style:style style:name="ce37" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #000000" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="end" fo:margin-left="0pt"/>
+    </style:style>
     <style:style style:name="ce19" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
     </style:style>
@@ -1153,7 +1157,7 @@
           <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="4">
             <text:p>Insert</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="4">
+          <table:table-cell table:style-name="ce37" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="4">
             <text:p>ID Sales &amp; ID Customer is foregin key</text:p>
           </table:table-cell>
           <table:table-cell/>
@@ -1287,9 +1291,9 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
     <meta:creation-date>2020-04-20T21:01:13.174337934</meta:creation-date>
-    <dc:date>2020-04-27T10:28:42.644529550</dc:date>
-    <meta:editing-duration>P2DT5M47S</meta:editing-duration>
-    <meta:editing-cycles>75</meta:editing-cycles>
+    <dc:date>2020-05-01T09:47:41.432848015</dc:date>
+    <meta:editing-duration>P4DT5H27M40S</meta:editing-duration>
+    <meta:editing-cycles>77</meta:editing-cycles>
     <meta:generator>LibreOffice/6.0.7.3$Linux_X86_64 LibreOffice_project/00m0$Build-3</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="226" meta:object-count="0"/>
   </office:meta>
@@ -1309,8 +1313,8 @@
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">48</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">65</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -1319,7 +1323,7 @@
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">13</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">36</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">81</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -1328,7 +1332,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Sheet1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1351</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1312</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">81</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -1360,7 +1364,7 @@
       <config:config-item config:name="IsKernAsianPunctuation" config:type="boolean">false</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">hQH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMApgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">kQH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAsgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item-map-indexed config:name="ForbiddenCharacters">
         <config:config-item-map-entry>
@@ -1524,9 +1528,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2020-04-27">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2020-05-01">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="11:40:05.928921285">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="03:55:35.907996890">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
create modul setoran hutang
</commit_message>
<xml_diff>
--- a/Raw Process New Modul_.xlsx
+++ b/Raw Process New Modul_.xlsx
@@ -55,6 +55,23 @@
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
+    <number:date-style style:name="N37" number:automatic-order="true">
+      <number:month number:style="long"/>
+      <number:text>/</number:text>
+      <number:day number:style="long"/>
+      <number:text>/</number:text>
+      <number:year/>
+    </number:date-style>
+    <number:number-style style:name="N106P0" style:volatile="true">
+      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N106">
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" loext:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N106P0"/>
+    </number:number-style>
     <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:border="none"/>
       <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
@@ -104,15 +121,17 @@
       <style:table-cell-properties fo:border="0.06pt solid #000000"/>
       <style:text-properties fo:font-weight="normal" style:font-weight-asian="normal" style:font-weight-complex="normal"/>
     </style:style>
-    <style:style style:name="ce32" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #000000" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0pt"/>
-    </style:style>
+    <style:style style:name="ce32" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N106"/>
     <style:style style:name="ce33" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #000000" style:vertical-align="middle"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0pt"/>
+    </style:style>
+    <style:style style:name="ce34" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #000000" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0pt"/>
       <style:text-properties fo:font-weight="normal" style:font-weight-asian="normal" style:font-weight-complex="normal"/>
     </style:style>
+    <style:style style:name="ce35" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N37"/>
     <style:style style:name="ce16" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:border-bottom="none" fo:border-left="none" fo:border-right="1.5pt solid #000000" fo:border-top="1.5pt solid #000000"/>
     </style:style>
@@ -142,16 +161,14 @@
     <office:spreadsheet>
       <table:calculation-settings table:automatic-find-labels="false" table:use-regular-expressions="false" table:use-wildcards="true"/>
       <table:table table:name="Sheet1" table:style-name="ta1">
+        <table:table-column table:style-name="co1" table:number-columns-repeated="2" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co3" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co1" table:default-cell-style-name="ce4"/>
-        <table:table-column table:style-name="co2" table:default-cell-style-name="ce28"/>
-        <table:table-column table:style-name="co3" table:default-cell-style-name="ce28"/>
-        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co4" table:default-cell-style-name="ce28"/>
-        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co1" table:default-cell-style-name="ce3"/>
-        <table:table-column table:style-name="co5" table:default-cell-style-name="ce28"/>
-        <table:table-column table:style-name="co6" table:default-cell-style-name="ce28"/>
+        <table:table-column table:style-name="co4" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="2" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co5" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co6" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co7" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co8" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co9" table:default-cell-style-name="Default"/>
@@ -161,8 +178,7 @@
           <table:table-cell table:style-name="ce7" table:number-columns-repeated="4"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce19"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell table:number-columns-repeated="3"/>
+          <table:table-cell table:number-columns-repeated="5"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
@@ -182,32 +198,15 @@
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
           <table:table-cell table:style-name="ce3"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>I</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
-            <text:p>Input Data</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
-            <text:p>Tipe Data</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
-            <text:p>Method</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
-            <text:p>Condition</text:p>
-          </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>I</text:p>
@@ -225,106 +224,122 @@
             <text:p>Condition</text:p>
           </table:table-cell>
           <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>I</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
+            <text:p>Input Data</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
+            <text:p>Tipe Data</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
+            <text:p>Method</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
+            <text:p>Condition</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Customer</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>AutoIncrement (int)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
             <text:p>Insert</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
             <text:p>No condition</text:p>
           </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce4"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Area</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Autoincrement (int)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
             <text:p>Insert</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
             <text:p>No condition</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Nama Customer</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce4"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Area</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Limit</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Longint</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce4"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = True</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Hutang</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Longint</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce4"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Alamat</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>II</text:p>
@@ -344,66 +359,66 @@
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>No Telp</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce4"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Area</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>Update</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>ID Area = param &amp; ID Area Not Exist in Modul Sales Mapping</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = True</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce4"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = True/False</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce4"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
           <table:table-cell table:style-name="ce11" table:number-columns-repeated="2"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce17"/>
@@ -426,7 +441,8 @@
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Edit Data</text:p>
           </table:table-cell>
@@ -441,53 +457,53 @@
           </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce4"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = False</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string">
             <text:p>Update</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string">
             <text:p>ID Area = param</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>II</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Nama Customer</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="6">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="6">
             <text:p>Update</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="6">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="6">
             <text:p>ID Customer = param</text:p>
           </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce4"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Limit</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Longint</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>IV</text:p>
@@ -507,86 +523,86 @@
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Hutang</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Longint</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Area</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Autoincrement (int)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>Select</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>Flagging = true</text:p>
           </table:table-cell>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Alamat</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce5"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Area</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>No Telp</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = True/False</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Hapus Data</text:p>
           </table:table-cell>
@@ -608,32 +624,33 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>III</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = False</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string">
             <text:p>Update</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce18" office:value-type="string" calcext:value-type="string">
             <text:p>ID Customer = param</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
           <table:table-cell table:style-name="ce19" table:number-columns-repeated="4"/>
           <table:table-cell table:style-name="ce21"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
           <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>I</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
@@ -653,7 +670,8 @@
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Tampil Data</text:p>
           </table:table-cell>
@@ -666,185 +684,183 @@
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Condition</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Setoran</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Autoincrement (int)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
             <text:p>Insert – Update</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
             <text:p>No condition</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
             <text:p>Decrease Hutang @ X01</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>IV</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Customer</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>AutoIncrement(int)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
             <text:p>Select</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
             <text:p>Flagging = true</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Mapping</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(int) → X04</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell table:style-name="ce32"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce3"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:style-name="ce33"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Nama Customer</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>ID Penjualan/ nofak</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Lookup(int) → Modul Jual</text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ID Penjualan</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Lookup(int) → Modul Jual</text:p>
-          </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Limit</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Longint</text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Setoran</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Longint</text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell table:style-name="ce32"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce3"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Limit</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:style-name="ce33"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Hutang</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Longint</text:p>
           </table:table-cell>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Flagging</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Boolean = True</text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Setoran</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Longint</text:p>
-          </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Alamat</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Varchar</text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Insert Tanggal Setoran</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>Datetime</text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell table:style-name="ce32"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce3"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Hutang</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Longint</text:p>
-          </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Flagging</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Boolean = True</text:p>
-          </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell table:style-name="ce32"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce3"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Alamat</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:style-name="ce33"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
+            <text:p>No Telp</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Insert Tanggal Setoran</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Datetime</text:p>
-          </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell table:style-name="ce32"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce3"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>No Telp</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Varchar</text:p>
-          </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Update Tanggal Setoran</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>Datetime</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
           <table:table-cell table:style-name="ce5"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = True</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce28"/>
-          <table:covered-table-cell/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="Default"/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce28"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell/>
           <table:table-cell table:style-name="ce20"/>
           <table:table-cell table:style-name="ce19" table:number-columns-repeated="2"/>
           <table:table-cell table:style-name="ce17"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default"/>
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:number-columns-repeated="7"/>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>II</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
@@ -864,24 +880,21 @@
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default"/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:number-columns-repeated="7"/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Setoran</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Autoincrement (int)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>Update</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>ID Setoran = param</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="2">
             <text:p>Increase Hutang with old value and Decrease Hutang with new value @ X01</text:p>
           </table:table-cell>
         </table:table-row>
@@ -894,16 +907,17 @@
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce5"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = False</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="3" table:style-name="ce32"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:covered-table-cell table:number-columns-repeated="3" table:style-name="ce33"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Input Data</text:p>
           </table:table-cell>
@@ -916,40 +930,37 @@
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Condition</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>I</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Sales</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>AutoIncrement(int)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
             <text:p>Insert</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
             <text:p>No condition</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Karyawan</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Varchar</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>Table Log Hutang</text:p>
@@ -959,15 +970,17 @@
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = True</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Column</text:p>
           </table:table-cell>
@@ -983,27 +996,29 @@
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
           <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>ID History</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>Autoincrement (int)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
+          <table:table-cell table:style-name="ce34" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
             <text:p>Insert</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
+          <table:table-cell table:style-name="ce34" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="7">
             <text:p>No condition</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce19"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Edit Data/Hapus Data</text:p>
           </table:table-cell>
@@ -1016,14 +1031,15 @@
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Condition</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Customer</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(int) → X01</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
           <table:table-cell/>
         </table:table-row>
@@ -1032,77 +1048,78 @@
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>II</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Flagging</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Boolean = False</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Update</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string">
             <text:p>ID Sales = param</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Sales</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(int) → X02</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
           <table:table-cell table:style-name="ce7"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce7"/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Penjualan</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(int) → Modul Jual</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
           <table:table-cell table:style-name="ce7"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce7"/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Setoran</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Longint</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
           <table:table-cell table:style-name="ce7"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce7"/>
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Hutang</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(int) → X01</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
           <table:table-cell/>
         </table:table-row>
@@ -1115,19 +1132,19 @@
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce5"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Insert Tanggal Setoran</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Datetime</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:style-name="ce32"/>
+          <table:covered-table-cell table:style-name="ce33"/>
           <table:covered-table-cell table:style-name="ce28"/>
           <table:table-cell/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>I</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -1142,79 +1159,71 @@
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Condition</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
           <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>ID Mapping</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>AutoIncrement (int)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="4">
+          <table:table-cell table:style-name="ce34" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="4">
             <text:p>Insert</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce37" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="4">
             <text:p>ID Sales &amp; ID Customer is foregin key</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Sales</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(int) →X02</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Customer</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(int) → X01</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Area</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(varchar) → X03</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="2"/>
-          <table:table-cell/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4"/>
+          <table:table-cell table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce17"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>II</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -1229,55 +1238,511 @@
           <table:table-cell table:style-name="ce9" office:value-type="string" calcext:value-type="string">
             <text:p>Condition</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce3"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Sales</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(int) → X02</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
             <text:p>Update</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
+          <table:table-cell table:style-name="ce33" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
             <text:p>ID Mapping = param</text:p>
           </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce3"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>ID Customer</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(int) → X01</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
-          <table:table-cell table:number-columns-repeated="3"/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell table:number-columns-repeated="7"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
           <table:table-cell table:style-name="ce5"/>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Area</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce28" office:value-type="string" calcext:value-type="string">
             <text:p>Lookup(varchar) → X03</text:p>
           </table:table-cell>
-          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce32"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="Default" table:number-columns-repeated="3"/>
+          <table:covered-table-cell table:number-columns-repeated="2" table:style-name="ce33"/>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="7">
+          <table:table-cell table:number-columns-repeated="13"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>No Faktur/ Nota</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="5"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Status Bayar</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="5"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Autocomplete</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="5"/>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="float" office:value="12345" calcext:value-type="float">
+            <text:p>12345</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="11"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Barang A</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="10" calcext:value-type="float">
+            <text:p>10</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="100000" calcext:value-type="float">
+            <text:p>100000</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1000000" calcext:value-type="float">
+            <text:p>1000000</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Barang B</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="4" calcext:value-type="float">
+            <text:p>4</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1000000" calcext:value-type="float">
+            <text:p>1000000</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="4000000" calcext:value-type="float">
+            <text:p>4000000</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="5">
+          <table:table-cell table:number-columns-repeated="13"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="4"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Total</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="5000000" calcext:value-type="float">
+            <text:p>5000000</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="4"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Sudah Bayar</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="5000000" calcext:value-type="float">
+            <text:p>5000000</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="4"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Bayar</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="13"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="4"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Simpan</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="8"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="4">
+          <table:table-cell table:number-columns-repeated="13"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Customer</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="11"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>PT. AKI CILEGON</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="11"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="13"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Total Hutang</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="5000000" calcext:value-type="float">
+            <text:p>5000000</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="9"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Bayar</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2000000" calcext:value-type="float">
+            <text:p>2000000</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="9"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="7">
+          <table:table-cell table:number-columns-repeated="13"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>PT. MAJU JAYA</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>-&gt; munculin data yang memiliki status bayar = 0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="9"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="13"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>No</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>No Faktur</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Total Hutang</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Bayar</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="8"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A01</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>5.000.000</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>3.000.000</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Tombol</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A02</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>7.000.000</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>4.000.000</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Tombol</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="7"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="2">
+          <table:table-cell table:number-columns-repeated="13"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Simpan</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="11"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Update data penjualan, update bagian status bayarnya menjadi 1 → JIKA total hutang dan total bayar ekuivalen</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="11"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="2">
+          <table:table-cell table:number-columns-repeated="13"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>id_setoran</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>nofak</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Total Belanja</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>tgl</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Setoran</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Sisa Hutang</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="5"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A01</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1800000" calcext:value-type="float">
+            <text:p>1,800,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce35" office:value-type="date" office:date-value="2020-05-07" calcext:value-type="date">
+            <text:p>05/07/20</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="100000" calcext:value-type="float">
+            <text:p>100,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1700000" calcext:value-type="float">
+            <text:p>1,700,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1800000" calcext:value-type="float">
+            <text:p>1,800,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A01</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1800000" calcext:value-type="float">
+            <text:p>1,800,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce35" office:value-type="date" office:date-value="2020-05-06" calcext:value-type="date">
+            <text:p>05/06/20</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="200000" calcext:value-type="float">
+            <text:p>200,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1500000" calcext:value-type="float">
+            <text:p>1,500,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1700000" calcext:value-type="float">
+            <text:p>1,700,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="float" office:value="3" calcext:value-type="float">
+            <text:p>3</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A01</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1800000" calcext:value-type="float">
+            <text:p>1,800,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce35" office:value-type="date" office:date-value="2020-05-08" calcext:value-type="date">
+            <text:p>05/08/20</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="500000" calcext:value-type="float">
+            <text:p>500,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1000000" calcext:value-type="float">
+            <text:p>1,000,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1500000" calcext:value-type="float">
+            <text:p>1,500,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="float" office:value="4" calcext:value-type="float">
+            <text:p>4</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A01</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1800000" calcext:value-type="float">
+            <text:p>1,800,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce35" office:value-type="date" office:date-value="2020-05-10" calcext:value-type="date">
+            <text:p>05/10/20</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1000000" calcext:value-type="float">
+            <text:p>1,000,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1000000" calcext:value-type="float">
+            <text:p>1,000,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="float" office:value="5" calcext:value-type="float">
+            <text:p>5</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A02</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="5000000" calcext:value-type="float">
+            <text:p>5,000,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce35" office:value-type="date" office:date-value="2020-05-11" calcext:value-type="date">
+            <text:p>05/11/20</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="3000000" calcext:value-type="float">
+            <text:p>3,000,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="2000000" calcext:value-type="float">
+            <text:p>2,000,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" table:number-columns-repeated="2"/>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="float" office:value="6" calcext:value-type="float">
+            <text:p>6</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A02</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="5000000" calcext:value-type="float">
+            <text:p>5,000,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce35" office:value-type="date" office:date-value="2020-05-12" calcext:value-type="date">
+            <text:p>05/12/20</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="2000000" calcext:value-type="float">
+            <text:p>2,000,000 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" table:number-columns-repeated="2"/>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="14">
+          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce32" table:number-columns-repeated="8"/>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string">
+            <text:p>Buat kolom temporary</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" table:number-columns-repeated="6"/>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce32" office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2 </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string">
+            <text:p>Ambil value yg dikurang dari sisa_hutang di id setoran sebelumnya yang memiliki no faktur yang sama</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" table:number-columns-repeated="6"/>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="4">
+          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce32" table:number-columns-repeated="8"/>
+          <table:table-cell table:number-columns-repeated="3"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="2"/>
+          <table:table-cell table:style-name="ce32"/>
+          <table:table-cell table:style-name="ce32" office:value-type="string" calcext:value-type="string">
+            <text:p>4 – 3</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce32" table:number-columns-repeated="6"/>
           <table:table-cell table:number-columns-repeated="3"/>
         </table:table-row>
       </table:table>
@@ -1291,11 +1756,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
     <meta:creation-date>2020-04-20T21:01:13.174337934</meta:creation-date>
-    <dc:date>2020-05-01T09:47:41.432848015</dc:date>
-    <meta:editing-duration>P4DT5H27M40S</meta:editing-duration>
-    <meta:editing-cycles>77</meta:editing-cycles>
+    <dc:date>2020-05-07T11:53:33.431442315</dc:date>
+    <meta:editing-duration>P4DT5H40M22S</meta:editing-duration>
+    <meta:editing-cycles>80</meta:editing-cycles>
     <meta:generator>LibreOffice/6.0.7.3$Linux_X86_64 LibreOffice_project/00m0$Build-3</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="226" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="324" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -1305,16 +1770,16 @@
   <office:settings>
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">903</config:config-item>
-      <config:config-item config:name="VisibleAreaLeft" config:type="int">2257</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">58461</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">24835</config:config-item>
+      <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">60718</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">59605</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">65</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">112</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -1323,7 +1788,7 @@
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">36</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">93</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">81</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -1364,7 +1829,7 @@
       <config:config-item config:name="IsKernAsianPunctuation" config:type="boolean">false</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">kQH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAsgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">kQH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAsgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKUGFnZVNpemU6QTQARHVwbGV4Ok5vbmUAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item-map-indexed config:name="ForbiddenCharacters">
         <config:config-item-map-entry>
@@ -1528,9 +1993,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2020-05-01">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2020-05-07">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="03:55:35.907996890">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="00:14:05.123833308">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>